<commit_message>
wrote reflection and test cases
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordicampoverde/PycharmProjects/cs151-lab4-jordi-and-megan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A5B61B2-3B1F-DB49-BA71-292F333B4D07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D99D52B-54E8-5E43-86D3-D97AACBB3249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="28800" windowHeight="18000" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="4" r:id="rId1"/>
@@ -439,7 +439,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>